<commit_message>
increased search space size
</commit_message>
<xml_diff>
--- a/experiment_list.xlsx
+++ b/experiment_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\OneDrive\DSTI\Courses\NC\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16896EA0-C6F6-436E-B0E1-6032EC96DA29}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B134BC2-6671-40CA-846F-5CEFC099523A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,16 +450,16 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>1000</v>
       </c>
       <c r="C2">
         <v>0.75</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -482,16 +482,16 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="C3">
         <v>0.75</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -514,16 +514,16 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="C4">
         <v>0.75</v>
       </c>
       <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
         <v>100</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
       </c>
       <c r="F4">
         <v>2</v>

</xml_diff>

<commit_message>
implemented using k1 and sqr
</commit_message>
<xml_diff>
--- a/experiment_list.xlsx
+++ b/experiment_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\OneDrive\DSTI\Courses\NC\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B134BC2-6671-40CA-846F-5CEFC099523A}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DEA5126-684B-4C78-9EFF-4F34166ED504}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>experiment_id</t>
   </si>
@@ -66,13 +66,7 @@
     <t>001</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>1,9</t>
+    <t>1,10</t>
   </si>
 </sst>
 </file>
@@ -400,7 +394,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,10 +444,10 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -465,81 +459,27 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J2">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>5000</v>
-      </c>
-      <c r="C3">
-        <v>0.75</v>
-      </c>
-      <c r="D3">
-        <v>500</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3">
-        <v>0.1</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>10000</v>
-      </c>
-      <c r="C4">
-        <v>0.75</v>
-      </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4">
-        <v>0.1</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
removed k1 and sqr
</commit_message>
<xml_diff>
--- a/experiment_list.xlsx
+++ b/experiment_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\OneDrive\DSTI\Courses\NC\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DEA5126-684B-4C78-9EFF-4F34166ED504}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EADD3D6-DE98-45DA-9E6F-D14CCE9A2639}"/>
   <bookViews>
     <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +444,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C2">
         <v>0.8</v>

</xml_diff>

<commit_message>
cleaned up comments, removed b
</commit_message>
<xml_diff>
--- a/experiment_list.xlsx
+++ b/experiment_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\OneDrive\DSTI\Courses\NC\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EADD3D6-DE98-45DA-9E6F-D14CCE9A2639}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="11_F25DC773A252ABDACC1048BFF15A42705BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{150B9D20-B435-4DE6-B345-C5E17862A96F}"/>
   <bookViews>
     <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>experiment_id</t>
   </si>
@@ -57,9 +57,6 @@
     <t>a_range</t>
   </si>
   <si>
-    <t>b_range</t>
-  </si>
-  <si>
     <t>p_mutate</t>
   </si>
   <si>
@@ -67,13 +64,31 @@
   </si>
   <si>
     <t>1,10</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +98,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,47 +428,44 @@
     <col min="3" max="3" width="11.6328125" customWidth="1"/>
     <col min="4" max="7" width="10.453125" customWidth="1"/>
     <col min="8" max="8" width="11.1796875" customWidth="1"/>
-    <col min="9" max="10" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>0.8</v>
@@ -462,27 +483,189 @@
         <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2">
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>0.8</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>0.8</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>0.8</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>0.8</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>0.8</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>